<commit_message>
FIX bugfixes with the performance test
</commit_message>
<xml_diff>
--- a/performance_report.xlsx
+++ b/performance_report.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Path" sheetId="1" r:id="rId1"/>
     <sheet name="DFS" sheetId="2" r:id="rId2"/>
+    <sheet name="Prim" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Execution time in relation to sidesteps done in a 10001x10001 grid when generating a random path</t>
   </si>
@@ -26,13 +27,16 @@
     <t>Height</t>
   </si>
   <si>
-    <t>steps required</t>
+    <t>Steps required</t>
   </si>
   <si>
     <t>Execution time</t>
   </si>
   <si>
     <t>Execution time in relation to the size of the maze when generating a maze using DFS</t>
+  </si>
+  <si>
+    <t>Execution time in relation to the size of the maze when generating a maze using PRIM</t>
   </si>
 </sst>
 </file>
@@ -111,10 +115,10 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Path!$C$4:$C$12</c:f>
+              <c:f>Path!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20000</c:v>
                 </c:pt>
@@ -140,6 +144,9 @@
                   <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>60000</c:v>
                 </c:pt>
               </c:numCache>
@@ -147,36 +154,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Path!$D$4:$D$12</c:f>
+              <c:f>Path!$D$4:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.1600282192230225</c:v>
+                  <c:v>0.2244138717651367</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.07354211807250977</c:v>
+                  <c:v>0.07827544212341309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1064772605895996</c:v>
+                  <c:v>0.1126272678375244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5371265411376953</c:v>
+                  <c:v>0.5410482883453369</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.430179357528687</c:v>
+                  <c:v>1.705308437347412</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.046423196792603</c:v>
+                  <c:v>3.676536798477173</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.5029878616333</c:v>
+                  <c:v>9.494065523147583</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.57518005371094</c:v>
+                  <c:v>16.90302324295044</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.38452911376953</c:v>
+                  <c:v>21.75908899307251</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.38172554969788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,10 +303,10 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>DFS!$C$4:$C$7</c:f>
+              <c:f>DFS!$C$4:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -308,27 +318,69 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>DFS!$D$4:$D$7</c:f>
+              <c:f>DFS!$D$4:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.367134094238281e-05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0002315044403076172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.004004716873168945</c:v>
+                  <c:v>0.003266096115112305</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01400184631347656</c:v>
+                  <c:v>0.01200366020202637</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.09736919403076172</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2840476036071777</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.298737287521362</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.476928472518921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.58010458946228</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>105.5442688465118</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>187.1719889640808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -413,6 +465,200 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="15"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution time in relation to the size of the maze when generating a maze using PRIM</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Prim!$C$4:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Prim!$D$4:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0001270771026611328</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0002923011779785156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.002956390380859375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01243448257446289</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1056084632873535</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.312997579574585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.36595344543457</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.619316816329956</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.97184109687805</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111.2998888492584</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>185.3081941604614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="50030001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of a side of the maze</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030002"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50030002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -449,6 +695,41 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -768,7 +1049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -804,7 +1085,7 @@
         <v>20000</v>
       </c>
       <c r="D4">
-        <v>0.1600282192230225</v>
+        <v>0.2244138717651367</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -818,7 +1099,7 @@
         <v>20004</v>
       </c>
       <c r="D5">
-        <v>0.07354211807250977</v>
+        <v>0.07827544212341309</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -832,7 +1113,7 @@
         <v>20040</v>
       </c>
       <c r="D6">
-        <v>0.1064772605895996</v>
+        <v>0.1126272678375244</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -846,7 +1127,7 @@
         <v>20400</v>
       </c>
       <c r="D7">
-        <v>0.5371265411376953</v>
+        <v>0.5410482883453369</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -860,7 +1141,7 @@
         <v>24000</v>
       </c>
       <c r="D8">
-        <v>2.430179357528687</v>
+        <v>1.705308437347412</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -874,7 +1155,7 @@
         <v>28000</v>
       </c>
       <c r="D9">
-        <v>5.046423196792603</v>
+        <v>3.676536798477173</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -888,7 +1169,7 @@
         <v>38000</v>
       </c>
       <c r="D10">
-        <v>13.5029878616333</v>
+        <v>9.494065523147583</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -902,7 +1183,7 @@
         <v>48000</v>
       </c>
       <c r="D11">
-        <v>22.57518005371094</v>
+        <v>16.90302324295044</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -913,10 +1194,24 @@
         <v>10001</v>
       </c>
       <c r="C12">
+        <v>55000</v>
+      </c>
+      <c r="D12">
+        <v>21.75908899307251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>10001</v>
+      </c>
+      <c r="B13">
+        <v>10001</v>
+      </c>
+      <c r="C13">
         <v>60000</v>
       </c>
-      <c r="D12">
-        <v>35.38452911376953</v>
+      <c r="D13">
+        <v>26.38172554969788</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +1222,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -963,7 +1258,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>7.367134094238281E-05</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -977,7 +1272,7 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.0002315044403076172</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -991,7 +1286,7 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <v>0.004004716873168945</v>
+        <v>0.003266096115112305</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1005,7 +1300,292 @@
         <v>200</v>
       </c>
       <c r="D7">
-        <v>0.01400184631347656</v>
+        <v>0.01200366020202637</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>301</v>
+      </c>
+      <c r="B8">
+        <v>301</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
+      </c>
+      <c r="D8">
+        <v>0.09736919403076172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>501</v>
+      </c>
+      <c r="B9">
+        <v>501</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>0.2840476036071777</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>1001</v>
+      </c>
+      <c r="B10">
+        <v>1001</v>
+      </c>
+      <c r="C10">
+        <v>2000</v>
+      </c>
+      <c r="D10">
+        <v>1.298737287521362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>2001</v>
+      </c>
+      <c r="B11">
+        <v>2001</v>
+      </c>
+      <c r="C11">
+        <v>4000</v>
+      </c>
+      <c r="D11">
+        <v>4.476928472518921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>5001</v>
+      </c>
+      <c r="B12">
+        <v>5001</v>
+      </c>
+      <c r="C12">
+        <v>10000</v>
+      </c>
+      <c r="D12">
+        <v>33.58010458946228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>8001</v>
+      </c>
+      <c r="B13">
+        <v>8001</v>
+      </c>
+      <c r="C13">
+        <v>16000</v>
+      </c>
+      <c r="D13">
+        <v>105.5442688465118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>10001</v>
+      </c>
+      <c r="B14">
+        <v>10001</v>
+      </c>
+      <c r="C14">
+        <v>20000</v>
+      </c>
+      <c r="D14">
+        <v>187.1719889640808</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>0.0001270771026611328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>0.0002923011779785156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>0.002956390380859375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>101</v>
+      </c>
+      <c r="B7">
+        <v>101</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>0.01243448257446289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>301</v>
+      </c>
+      <c r="B8">
+        <v>301</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
+      </c>
+      <c r="D8">
+        <v>0.1056084632873535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>501</v>
+      </c>
+      <c r="B9">
+        <v>501</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>0.312997579574585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>1001</v>
+      </c>
+      <c r="B10">
+        <v>1001</v>
+      </c>
+      <c r="C10">
+        <v>2000</v>
+      </c>
+      <c r="D10">
+        <v>1.36595344543457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>2001</v>
+      </c>
+      <c r="B11">
+        <v>2001</v>
+      </c>
+      <c r="C11">
+        <v>4000</v>
+      </c>
+      <c r="D11">
+        <v>5.619316816329956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>5001</v>
+      </c>
+      <c r="B12">
+        <v>5001</v>
+      </c>
+      <c r="C12">
+        <v>10000</v>
+      </c>
+      <c r="D12">
+        <v>38.97184109687805</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>8001</v>
+      </c>
+      <c r="B13">
+        <v>8001</v>
+      </c>
+      <c r="C13">
+        <v>16000</v>
+      </c>
+      <c r="D13">
+        <v>111.2998888492584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>10001</v>
+      </c>
+      <c r="B14">
+        <v>10001</v>
+      </c>
+      <c r="C14">
+        <v>20000</v>
+      </c>
+      <c r="D14">
+        <v>185.3081941604614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>